<commit_message>
WIP implementation of Conv1D.
</commit_message>
<xml_diff>
--- a/out/scores.xlsx
+++ b/out/scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Colin/PycharmProjects/mmai823-project/out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7AE23D-BB25-034D-AA30-B355834F983A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD33A98-B259-8943-A7F9-64C37C626156}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rf_scores" sheetId="1" r:id="rId1"/>
@@ -706,7 +706,97 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -765,7 +855,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Model AUC Scores by Commodity</a:t>
+              <a:t>Model Accuracy Scores by Commodity</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1661,6 +1751,95 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-2AD1-5B4D-BB8B-658E00F3DBAE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>rf_scores!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>score_conv1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>rf_scores!$I$2:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.294573634862899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.341085284948349</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.198966413736343</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33333334326744002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30490955710411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30490955710411</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.31266149878501798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.30490955710411</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.62532299757003695</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.67183464765548695</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.62015503644943204</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.67441862821578902</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.65891474485397294</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.66925066709518399</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.66666668653488104</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.66408270597457797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4EB3-4647-A46F-C285A01E971B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2415,16 +2594,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>29826</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>29825</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>112376</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>112375</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>97303</xdr:rowOff>
+      <xdr:rowOff>97304</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2776,7 +2955,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2846,8 +3025,8 @@
         <v>0.294573634862899</v>
       </c>
       <c r="J2">
-        <f>AVERAGE(C2:H2)</f>
-        <v>0.33195753935102262</v>
+        <f>AVERAGE(C2:I2)</f>
+        <v>0.32661698156700497</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2879,8 +3058,8 @@
         <v>0.341085284948349</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J17" si="0">AVERAGE(C3:H3)</f>
-        <v>0.29046416546416493</v>
+        <f t="shared" ref="J3:J17" si="0">AVERAGE(C3:I3)</f>
+        <v>0.29769575396190551</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2913,7 +3092,7 @@
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0.329076745823288</v>
+        <v>0.310489555525153</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2946,7 +3125,7 @@
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>0.33790504852871023</v>
+        <v>0.33725194777710016</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2979,7 +3158,7 @@
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>0.34534578603638599</v>
+        <v>0.33956918190320368</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3012,7 +3191,7 @@
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>0.34126429188520085</v>
+        <v>0.33607075834504496</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3045,7 +3224,7 @@
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>0.31756971581018434</v>
+        <v>0.31686854194944625</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3078,7 +3257,7 @@
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0.34126429188520085</v>
+        <v>0.33607075834504496</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3111,7 +3290,7 @@
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>0.49782939108957863</v>
+        <v>0.51604276344392985</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3144,7 +3323,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>0.50632192610539029</v>
+        <v>0.52996660061254697</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3177,7 +3356,7 @@
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>0.49980867346938718</v>
+        <v>0.51700101103796503</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3210,7 +3389,7 @@
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0.52066228790366686</v>
+        <v>0.5426274793768272</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3243,7 +3422,7 @@
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0.51042780748663052</v>
+        <v>0.5316402271105366</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3276,7 +3455,7 @@
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0.48496571348133805</v>
+        <v>0.51129213542617313</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3309,7 +3488,7 @@
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>0.49580103359173067</v>
+        <v>0.52021041258360934</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3342,15 +3521,39 @@
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>0.52101666167813987</v>
+        <v>0.54145466800620246</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J17">
-    <cfRule type="top10" dxfId="0" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:J17">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J17">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J9">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3361,17 +3564,26 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
+  <conditionalFormatting sqref="I10:I17">
+    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:H17">
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10:G17">
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:F17">
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E17">
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D17">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:C17">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>